<commit_message>
Updating Latex TOG and information
</commit_message>
<xml_diff>
--- a/03_IDI/IDI_II/Plan de Trabajo TOG_2.0.xlsx
+++ b/03_IDI/IDI_II/Plan de Trabajo TOG_2.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvjlu\Documents\02_Maestria\TOG\03_IDI\IDI_II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD89E6D-1539-4DC1-BDD7-F8F60946209D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C56333-8C4E-45D7-AB55-313B05A01A77}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4740" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TASKS" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Tarea</t>
   </si>
@@ -175,6 +173,9 @@
   </si>
   <si>
     <t>Estado del Arte Avances 2</t>
+  </si>
+  <si>
+    <t>Entregables</t>
   </si>
 </sst>
 </file>
@@ -310,7 +311,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -359,35 +360,38 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="5" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="4" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="16" fontId="6" fillId="5" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="16" fontId="6" fillId="4" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -400,11 +404,7 @@
     <cellStyle name="Table Text" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <numFmt numFmtId="21" formatCode="dd\-mmm"/>
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="30">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -464,6 +464,13 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="dd\-mmm"/>
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -577,10 +584,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Task List" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Task List" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="28"/>
-      <tableStyleElement type="headerRow" dxfId="27"/>
-      <tableStyleElement type="totalRow" dxfId="26"/>
-      <tableStyleElement type="firstColumn" dxfId="25"/>
+      <tableStyleElement type="wholeTable" dxfId="29"/>
+      <tableStyleElement type="headerRow" dxfId="28"/>
+      <tableStyleElement type="totalRow" dxfId="27"/>
+      <tableStyleElement type="firstColumn" dxfId="26"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -595,17 +602,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tasks" displayName="Tasks" ref="B2:G14" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tasks" displayName="Tasks" ref="B2:G14" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="B2:G14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tarea" dataDxfId="22" dataCellStyle="Table Text"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Fecha Planeada" dataDxfId="21" dataCellStyle="Date"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Fecha de Entrega" dataDxfId="20" dataCellStyle="Date"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="% Completado" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Hito" dataDxfId="18" dataCellStyle="Done">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tarea" dataDxfId="23" dataCellStyle="Table Text"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Fecha Planeada" dataDxfId="22" dataCellStyle="Date"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Fecha de Entrega" dataDxfId="21" dataCellStyle="Date"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="% Completado" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Hito" dataDxfId="19" dataCellStyle="Done">
       <calculatedColumnFormula>--(Tasks[[#This Row],[% Completado]]&gt;=1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Notas" dataDxfId="17" dataCellStyle="Table Text"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Notas" dataDxfId="18" dataCellStyle="Table Text"/>
   </tableColumns>
   <tableStyleInfo name="Task List" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -617,24 +624,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D5D23EDA-13DE-439E-ACDF-9F8D0FB2DC4F}" name="Tabla2" displayName="Tabla2" ref="B1:P13" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowCellStyle="Normal 2" dataCellStyle="Normal 2">
-  <autoFilter ref="B1:P13" xr:uid="{408CA22D-807B-4891-A5E8-D52B9A14D050}"/>
-  <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{9B59DE68-AB9A-41EE-A2F0-AA89A592E957}" name="#" dataDxfId="16" dataCellStyle="Normal 2"/>
-    <tableColumn id="2" xr3:uid="{1D7413CC-58C2-4F04-9440-D71D563041C0}" name="Entregable" dataDxfId="15" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{A60EB099-7954-405D-AE6C-7EF3078FFA29}" name="24-Feb" dataDxfId="14" dataCellStyle="Normal 2"/>
-    <tableColumn id="4" xr3:uid="{A76E44BF-28BC-421E-B28A-6E579AEB0530}" name="02-Mar" dataDxfId="13" dataCellStyle="Normal 2"/>
-    <tableColumn id="5" xr3:uid="{D28C99E4-3322-4F74-9EE6-AE3039716938}" name="09-Mar" dataDxfId="12" dataCellStyle="Normal 2"/>
-    <tableColumn id="6" xr3:uid="{3055C2B2-A30B-492B-9394-8E18F7DA0F7F}" name="16-Mar" dataDxfId="11" dataCellStyle="Normal 2"/>
-    <tableColumn id="7" xr3:uid="{7387D548-1031-46F6-BC16-7EFA3BECEE2D}" name="23-Mar" dataDxfId="10" dataCellStyle="Normal 2"/>
-    <tableColumn id="8" xr3:uid="{019DCF9A-97CA-4B48-88EE-ACDE66202019}" name="30-Mar" dataDxfId="9" dataCellStyle="Normal 2"/>
-    <tableColumn id="9" xr3:uid="{85D79B75-CC93-4168-89B4-D3093DB5D5B5}" name="06-Apr" dataDxfId="8" dataCellStyle="Normal 2"/>
-    <tableColumn id="10" xr3:uid="{8CFB39D4-A95A-44AC-B148-4BDA00A2D923}" name="13-Apr" dataDxfId="7" dataCellStyle="Normal 2"/>
-    <tableColumn id="11" xr3:uid="{46947C2F-7E3F-438E-927F-33BB97CE8B9A}" name="20-Apr" dataDxfId="6" dataCellStyle="Normal 2"/>
-    <tableColumn id="12" xr3:uid="{6960609C-DBA8-4008-86A8-8EA9F63B659F}" name="27-Apr" dataDxfId="5" dataCellStyle="Normal 2"/>
-    <tableColumn id="13" xr3:uid="{C388461D-4BF2-41B9-B879-EE91C91352D8}" name="04-May" dataDxfId="4" dataCellStyle="Normal 2"/>
-    <tableColumn id="14" xr3:uid="{E8E38311-3307-4D22-9158-410FA062B22C}" name="11-May" dataDxfId="3" dataCellStyle="Normal 2"/>
-    <tableColumn id="15" xr3:uid="{EE465099-B1D1-46EF-9CA4-90AC214D7927}" name="18-May" dataDxfId="2" dataCellStyle="Normal 2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D5D23EDA-13DE-439E-ACDF-9F8D0FB2DC4F}" name="Tabla2" displayName="Tabla2" ref="B1:Q13" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" headerRowCellStyle="Normal 2" dataCellStyle="Normal 2">
+  <autoFilter ref="B1:Q13" xr:uid="{408CA22D-807B-4891-A5E8-D52B9A14D050}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{9B59DE68-AB9A-41EE-A2F0-AA89A592E957}" name="#" dataDxfId="15" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{1D7413CC-58C2-4F04-9440-D71D563041C0}" name="Entregable" dataDxfId="14" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{A60EB099-7954-405D-AE6C-7EF3078FFA29}" name="24-Feb" dataDxfId="13" dataCellStyle="Normal 2"/>
+    <tableColumn id="4" xr3:uid="{A76E44BF-28BC-421E-B28A-6E579AEB0530}" name="02-Mar" dataDxfId="12" dataCellStyle="Normal 2"/>
+    <tableColumn id="5" xr3:uid="{D28C99E4-3322-4F74-9EE6-AE3039716938}" name="09-Mar" dataDxfId="11" dataCellStyle="Normal 2"/>
+    <tableColumn id="6" xr3:uid="{3055C2B2-A30B-492B-9394-8E18F7DA0F7F}" name="16-Mar" dataDxfId="10" dataCellStyle="Normal 2"/>
+    <tableColumn id="7" xr3:uid="{7387D548-1031-46F6-BC16-7EFA3BECEE2D}" name="23-Mar" dataDxfId="9" dataCellStyle="Normal 2"/>
+    <tableColumn id="8" xr3:uid="{019DCF9A-97CA-4B48-88EE-ACDE66202019}" name="30-Mar" dataDxfId="8" dataCellStyle="Normal 2"/>
+    <tableColumn id="9" xr3:uid="{85D79B75-CC93-4168-89B4-D3093DB5D5B5}" name="06-Apr" dataDxfId="7" dataCellStyle="Normal 2"/>
+    <tableColumn id="10" xr3:uid="{8CFB39D4-A95A-44AC-B148-4BDA00A2D923}" name="13-Apr" dataDxfId="6" dataCellStyle="Normal 2"/>
+    <tableColumn id="11" xr3:uid="{46947C2F-7E3F-438E-927F-33BB97CE8B9A}" name="20-Apr" dataDxfId="5" dataCellStyle="Normal 2"/>
+    <tableColumn id="12" xr3:uid="{6960609C-DBA8-4008-86A8-8EA9F63B659F}" name="27-Apr" dataDxfId="4" dataCellStyle="Normal 2"/>
+    <tableColumn id="13" xr3:uid="{C388461D-4BF2-41B9-B879-EE91C91352D8}" name="04-May" dataDxfId="3" dataCellStyle="Normal 2"/>
+    <tableColumn id="14" xr3:uid="{E8E38311-3307-4D22-9158-410FA062B22C}" name="11-May" dataDxfId="2" dataCellStyle="Normal 2"/>
+    <tableColumn id="15" xr3:uid="{EE465099-B1D1-46EF-9CA4-90AC214D7927}" name="18-May" dataDxfId="1" dataCellStyle="Normal 2"/>
+    <tableColumn id="16" xr3:uid="{B14AE06F-0C63-4DE7-90A9-9C7CD189C1B2}" name="Entregables" dataDxfId="0" dataCellStyle="Normal 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -866,14 +874,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -1175,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA31B94-7D8B-4D88-B9A2-7F30F0BAF654}">
-  <dimension ref="B1:P13"/>
+  <dimension ref="B1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1187,306 +1195,323 @@
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
     <col min="5" max="5" width="7.140625" customWidth="1"/>
     <col min="6" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="34.140625" customWidth="1"/>
+    <col min="18" max="18" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="42" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
+    <row r="1" spans="2:17" ht="65.25" x14ac:dyDescent="0.25">
+      <c r="B1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="P1" s="19" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="17">
+      <c r="Q1" s="26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="16">
         <v>1</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="23"/>
-    </row>
-    <row r="3" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="17">
+      <c r="D2" s="20"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="24"/>
+    </row>
+    <row r="3" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="16">
         <v>2</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="23"/>
-    </row>
-    <row r="4" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="17">
+      <c r="D3" s="20"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="24"/>
+    </row>
+    <row r="4" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="16">
         <v>3</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="23"/>
-    </row>
-    <row r="5" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="17">
+      <c r="D4" s="16"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="24"/>
+    </row>
+    <row r="5" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="16">
         <v>4</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="23"/>
-    </row>
-    <row r="6" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="17">
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="24"/>
+    </row>
+    <row r="6" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="16">
         <v>5</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="23"/>
-    </row>
-    <row r="7" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="17">
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="24"/>
+    </row>
+    <row r="7" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="16">
         <v>6</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="23"/>
-    </row>
-    <row r="8" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="17">
+      <c r="D7" s="16"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="24"/>
+    </row>
+    <row r="8" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="16">
         <v>7</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="23"/>
-    </row>
-    <row r="9" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="17">
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="24"/>
+    </row>
+    <row r="9" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="16">
         <v>8</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="23"/>
-    </row>
-    <row r="10" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="17">
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="24"/>
+    </row>
+    <row r="10" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="16">
         <v>9</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="23"/>
-    </row>
-    <row r="11" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="17">
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="24"/>
+    </row>
+    <row r="11" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="16">
         <v>10</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="23"/>
-    </row>
-    <row r="12" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="17">
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="24"/>
+    </row>
+    <row r="12" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="16">
         <v>11</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="23"/>
-    </row>
-    <row r="13" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="17">
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="24"/>
+    </row>
+    <row r="13" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="16">
         <v>12</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="23"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>